<commit_message>
new activity log, project2.asm to main folder
</commit_message>
<xml_diff>
--- a/OMEGA/Activity Log.xlsx
+++ b/OMEGA/Activity Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkbo\Desktop\Hex-Decoder\OMEGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rremi\Desktop\ECE 366\Hex-Decoder\OMEGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C22569A-FC93-47E3-A42F-3143568DBB8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E52660B-E10A-41E2-9D1D-A30318FC095D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
+    <workbookView xWindow="-1236" yWindow="1824" windowWidth="17280" windowHeight="8964" xr2:uid="{0F5DC705-85FB-4EAC-8F72-74DC7DEA8333}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,20 +524,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CA3FDB-D763-4CE5-9DE9-DF6F5D651576}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.08984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="1"/>
+    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -565,7 +565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -593,7 +593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -607,7 +607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -621,7 +621,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -635,7 +635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -649,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -663,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -677,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -691,7 +691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -705,7 +705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -719,7 +719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>

</xml_diff>